<commit_message>
Updated App with Instructions as first tab. Fixed issues with multiple curves being returned
</commit_message>
<xml_diff>
--- a/data/AdminData.xlsx
+++ b/data/AdminData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Paul\Documents\Data_Science_Spec\CampaignPlanning\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Paul\Documents\Data_Science_Spec\CampaignPlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="DatePeriods" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Reporting Period</t>
-  </si>
-  <si>
-    <t>2017 Q1</t>
   </si>
   <si>
     <t>Start</t>
@@ -41,37 +38,7 @@
     <t>End</t>
   </si>
   <si>
-    <t>2017 Q2</t>
-  </si>
-  <si>
     <t>2017 Q3</t>
-  </si>
-  <si>
-    <t>2017 Q4</t>
-  </si>
-  <si>
-    <t>2018 Q1</t>
-  </si>
-  <si>
-    <t>2018 Q2</t>
-  </si>
-  <si>
-    <t>2018 Q3</t>
-  </si>
-  <si>
-    <t>2018 Q4</t>
-  </si>
-  <si>
-    <t>2019 Q1</t>
-  </si>
-  <si>
-    <t>2019 Q2</t>
-  </si>
-  <si>
-    <t>2019 Q3</t>
-  </si>
-  <si>
-    <t>2019 Q4</t>
   </si>
   <si>
     <t>Func</t>
@@ -86,58 +53,13 @@
     <t>Area2</t>
   </si>
   <si>
-    <t>Area3</t>
-  </si>
-  <si>
-    <t>Area4</t>
-  </si>
-  <si>
-    <t>Area5</t>
-  </si>
-  <si>
     <t>Sub1</t>
   </si>
   <si>
     <t>Sub2</t>
   </si>
   <si>
-    <t>Sub3</t>
-  </si>
-  <si>
-    <t>Sub4</t>
-  </si>
-  <si>
-    <t>Sub5</t>
-  </si>
-  <si>
     <t>Sub6</t>
-  </si>
-  <si>
-    <t>Sub7</t>
-  </si>
-  <si>
-    <t>Sub8</t>
-  </si>
-  <si>
-    <t>Sub9</t>
-  </si>
-  <si>
-    <t>Sub10</t>
-  </si>
-  <si>
-    <t>Sub11</t>
-  </si>
-  <si>
-    <t>Sub12</t>
-  </si>
-  <si>
-    <t>Sub13</t>
-  </si>
-  <si>
-    <t>Sub14</t>
-  </si>
-  <si>
-    <t>Sub15</t>
   </si>
   <si>
     <t>Rday</t>
@@ -508,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,146 +447,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>42826</v>
+        <v>43009</v>
       </c>
       <c r="C2" s="1">
-        <v>42916</v>
+        <v>43100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>42917</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43008</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43009</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43101</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43191</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43281</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43282</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43373</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43374</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43465</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43466</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43556</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43646</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>43647</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43738</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43739</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>43831</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43921</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -673,140 +474,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -829,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -2674,46 +2379,80 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>